<commit_message>
add icon column in XLS gg-pin-blue gg-pin-pink gg-pin-green
</commit_message>
<xml_diff>
--- a/xls/geo-test.xlsx
+++ b/xls/geo-test.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
   <si>
     <t>x</t>
   </si>
@@ -94,6 +94,18 @@
   </si>
   <si>
     <t>จจจ</t>
+  </si>
+  <si>
+    <t>icon</t>
+  </si>
+  <si>
+    <t>gg-pin-blue</t>
+  </si>
+  <si>
+    <t>gg-pin-pink</t>
+  </si>
+  <si>
+    <t>gg-pin-green</t>
   </si>
 </sst>
 </file>
@@ -431,15 +443,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -458,8 +473,11 @@
       <c r="F1" t="s">
         <v>15</v>
       </c>
+      <c r="G1" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A2">
         <v>100</v>
       </c>
@@ -478,8 +496,11 @@
       <c r="F2" t="s">
         <v>21</v>
       </c>
+      <c r="G2" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>101</v>
       </c>
@@ -498,8 +519,11 @@
       <c r="F3" t="s">
         <v>22</v>
       </c>
+      <c r="G3" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>102</v>
       </c>
@@ -518,8 +542,11 @@
       <c r="F4" t="s">
         <v>23</v>
       </c>
+      <c r="G4" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>103</v>
       </c>
@@ -538,8 +565,11 @@
       <c r="F5" t="s">
         <v>24</v>
       </c>
+      <c r="G5" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>104</v>
       </c>
@@ -557,6 +587,9 @@
       </c>
       <c r="F6" t="s">
         <v>25</v>
+      </c>
+      <c r="G6" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add load xml and display features with icons on map
</commit_message>
<xml_diff>
--- a/xls/geo-test.xlsx
+++ b/xls/geo-test.xlsx
@@ -445,9 +445,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.4"/>
   <cols>

</xml_diff>